<commit_message>
fill template with 2019
</commit_message>
<xml_diff>
--- a/src/main/resources/f10-template.xlsx
+++ b/src/main/resources/f10-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ZE" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,8 +16,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">ZE!$A$1:$L$86</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'ZE-Sum'!$A$1:$O$61</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">ZE!$A$1:$L$86</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">ZE!$A$1:$L$86</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ZE!$A$7:$L$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'ZE-Sum'!$A$1:$O$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'ZE-Sum'!$A$1:$O$61</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -68,17 +70,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
-    <numFmt numFmtId="166" formatCode="00"/>
-    <numFmt numFmtId="167" formatCode="DDD"/>
-    <numFmt numFmtId="168" formatCode="D\-MMM"/>
-    <numFmt numFmtId="169" formatCode="H:MM"/>
-    <numFmt numFmtId="170" formatCode="0.00"/>
-    <numFmt numFmtId="171" formatCode="000,000"/>
-    <numFmt numFmtId="172" formatCode="0"/>
-    <numFmt numFmtId="173" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="00"/>
+    <numFmt numFmtId="166" formatCode="DDD"/>
+    <numFmt numFmtId="167" formatCode="D\-MMM"/>
+    <numFmt numFmtId="168" formatCode="H:MM"/>
+    <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="170" formatCode="000,000"/>
+    <numFmt numFmtId="171" formatCode="0"/>
+    <numFmt numFmtId="172" formatCode="@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -655,7 +656,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -679,11 +680,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="182">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,7 +742,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -852,7 +850,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -860,35 +862,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -916,11 +914,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -944,7 +942,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1032,35 +1030,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1068,19 +1066,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1088,10 +1086,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="true"/>
@@ -1104,27 +1098,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1144,147 +1138,147 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1340,11 +1334,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="2" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="2" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1368,63 +1362,62 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="3" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="14" fillId="3" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="14" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="14" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="14" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Euro" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1500,9 +1493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>637920</xdr:colOff>
+      <xdr:colOff>637560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>333000</xdr:rowOff>
+      <xdr:rowOff>332640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1515,8 +1508,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14593320" y="142920"/>
-          <a:ext cx="1811520" cy="485280"/>
+          <a:off x="14401800" y="142920"/>
+          <a:ext cx="1789920" cy="484920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1535,20 +1528,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>485640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>-11796120</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7560</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>332640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr=""/>
+        <xdr:cNvPr id="1" name="Picture 5" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1557,45 +1550,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="360000" cy="761400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>485640</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>333000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 5" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13644000" y="142920"/>
-          <a:ext cx="1681920" cy="485280"/>
+          <a:off x="13477680" y="142920"/>
+          <a:ext cx="1665000" cy="484920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1621,13 +1577,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>647280</xdr:colOff>
+      <xdr:colOff>646920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>275760</xdr:rowOff>
+      <xdr:rowOff>275400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 1" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1636,8 +1592,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6041160" y="85680"/>
-          <a:ext cx="1245960" cy="485280"/>
+          <a:off x="5962320" y="85680"/>
+          <a:ext cx="1237680" cy="484920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1662,29 +1618,29 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="9.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="43.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="93.5663265306122"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.9897959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.63265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="4.75"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.8979591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.4489795918367"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="1" width="9.69897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="24" style="1" width="4.61734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="9.69897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="92.4693877551021"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="32" min="24" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1701,7 +1657,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="4" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="6"/>
@@ -6866,7 +6822,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M8:M84" type="list">
-      <formula1>"X,"</formula1>
+      <formula1>"X"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -6896,26 +6852,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.95408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.77040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="45.6632653061225"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="4.61734693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="4.94897959183674"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="20" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="5.63265306122449"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="4.75"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.8979591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="10.4489795918367"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="9.69897959183673"/>
-    <col collapsed="false" hidden="false" max="37" min="29" style="1" width="4.61734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="9.69897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="45.2244897959184"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="22" min="20" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="37" min="29" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10278,7 +10234,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="101"/>
+      <c r="A11" s="87"/>
       <c r="B11" s="88"/>
       <c r="C11" s="89"/>
       <c r="D11" s="90" t="str">
@@ -10326,7 +10282,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="101"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="88"/>
       <c r="C12" s="89"/>
       <c r="D12" s="90" t="str">
@@ -10352,7 +10308,7 @@
       <c r="J12" s="94" t="n">
         <v>2450</v>
       </c>
-      <c r="K12" s="102" t="str">
+      <c r="K12" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Weiterbildung",IF(ZE!C3="EN","Further education","---"))</f>
         <v>Weiterbildung</v>
       </c>
@@ -10374,7 +10330,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="101"/>
+      <c r="A13" s="87"/>
       <c r="B13" s="88"/>
       <c r="C13" s="89"/>
       <c r="D13" s="90" t="str">
@@ -10400,7 +10356,7 @@
       <c r="J13" s="94" t="n">
         <v>2510</v>
       </c>
-      <c r="K13" s="102" t="str">
+      <c r="K13" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Ausbildung Intern",IF(ZE!C3="EN","Internal education","---"))</f>
         <v>Ausbildung Intern</v>
       </c>
@@ -10422,7 +10378,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="101"/>
+      <c r="A14" s="87"/>
       <c r="B14" s="88"/>
       <c r="C14" s="89"/>
       <c r="D14" s="90" t="str">
@@ -10448,7 +10404,7 @@
       <c r="J14" s="94" t="n">
         <v>2520</v>
       </c>
-      <c r="K14" s="102" t="str">
+      <c r="K14" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Leerkapazität",IF(ZE!C3="EN","Empty capacity","---"))</f>
         <v>Leerkapazität</v>
       </c>
@@ -10470,7 +10426,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="101"/>
+      <c r="A15" s="87"/>
       <c r="B15" s="88"/>
       <c r="C15" s="89"/>
       <c r="D15" s="90" t="str">
@@ -10496,7 +10452,7 @@
       <c r="J15" s="94" t="n">
         <v>2530</v>
       </c>
-      <c r="K15" s="102" t="str">
+      <c r="K15" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Interne Arbeiten",IF(ZE!C3="EN","Internal works","---"))</f>
         <v>Interne Arbeiten</v>
       </c>
@@ -10518,7 +10474,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="101"/>
+      <c r="A16" s="87"/>
       <c r="B16" s="88"/>
       <c r="C16" s="89"/>
       <c r="D16" s="90" t="str">
@@ -10542,7 +10498,7 @@
         <v> </v>
       </c>
       <c r="J16" s="94"/>
-      <c r="K16" s="103"/>
+      <c r="K16" s="102"/>
       <c r="L16" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J16,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J16,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -10558,7 +10514,7 @@
       <c r="O16" s="99"/>
     </row>
     <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="101"/>
+      <c r="A17" s="87"/>
       <c r="B17" s="88"/>
       <c r="C17" s="89"/>
       <c r="D17" s="90" t="str">
@@ -10584,7 +10540,7 @@
       <c r="J17" s="94" t="n">
         <v>3100</v>
       </c>
-      <c r="K17" s="102" t="str">
+      <c r="K17" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Marketing Allgemein",IF(ZE!C3="EN","General Marketing","---"))</f>
         <v>Marketing Allgemein</v>
       </c>
@@ -10606,7 +10562,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="101"/>
+      <c r="A18" s="87"/>
       <c r="B18" s="88"/>
       <c r="C18" s="89"/>
       <c r="D18" s="90" t="str">
@@ -10632,7 +10588,7 @@
       <c r="J18" s="94" t="n">
         <v>3201</v>
       </c>
-      <c r="K18" s="102" t="str">
+      <c r="K18" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","SAP Versicherungstage",IF(ZE!C3="EN","SAP Insurance Days","---"))</f>
         <v>SAP Versicherungstage</v>
       </c>
@@ -10654,7 +10610,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="101"/>
+      <c r="A19" s="87"/>
       <c r="B19" s="88"/>
       <c r="C19" s="89"/>
       <c r="D19" s="90" t="str">
@@ -10677,8 +10633,8 @@
         <f aca="false">G19</f>
         <v> </v>
       </c>
-      <c r="J19" s="101"/>
-      <c r="K19" s="103"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="102"/>
       <c r="L19" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J19,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J19,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -10697,7 +10653,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="101"/>
+      <c r="A20" s="87"/>
       <c r="B20" s="88"/>
       <c r="C20" s="89"/>
       <c r="D20" s="90" t="str">
@@ -10720,10 +10676,10 @@
         <f aca="false">G20</f>
         <v> </v>
       </c>
-      <c r="J20" s="101" t="n">
+      <c r="J20" s="87" t="n">
         <v>4200</v>
       </c>
-      <c r="K20" s="102" t="str">
+      <c r="K20" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","ConVista Köln",IF(ZE!C3="EN","ConVista Cologne","---"))</f>
         <v>ConVista Köln</v>
       </c>
@@ -10745,7 +10701,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="101"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="88"/>
       <c r="C21" s="89"/>
       <c r="D21" s="90" t="str">
@@ -10768,10 +10724,10 @@
         <f aca="false">G21</f>
         <v> </v>
       </c>
-      <c r="J21" s="101" t="n">
+      <c r="J21" s="87" t="n">
         <v>4300</v>
       </c>
-      <c r="K21" s="102" t="str">
+      <c r="K21" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","ConVista Hamburg",IF(ZE!C3="EN","ConVista Hamburg","---"))</f>
         <v>ConVista Hamburg</v>
       </c>
@@ -10793,7 +10749,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="101"/>
+      <c r="A22" s="87"/>
       <c r="B22" s="88"/>
       <c r="C22" s="89"/>
       <c r="D22" s="90" t="str">
@@ -10816,10 +10772,10 @@
         <f aca="false">G22</f>
         <v> </v>
       </c>
-      <c r="J22" s="101" t="n">
+      <c r="J22" s="87" t="n">
         <v>4400</v>
       </c>
-      <c r="K22" s="102" t="str">
+      <c r="K22" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","ConVista München",IF(ZE!C3="EN","ConVista Munich","---"))</f>
         <v>ConVista München</v>
       </c>
@@ -10841,7 +10797,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="101"/>
+      <c r="A23" s="87"/>
       <c r="B23" s="88"/>
       <c r="C23" s="89"/>
       <c r="D23" s="90" t="str">
@@ -10864,10 +10820,10 @@
         <f aca="false">G23</f>
         <v> </v>
       </c>
-      <c r="J23" s="101" t="n">
+      <c r="J23" s="87" t="n">
         <v>4500</v>
       </c>
-      <c r="K23" s="102" t="str">
+      <c r="K23" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","ConVista Schweiz",IF(ZE!C3="EN","ConVista Switzerland","---"))</f>
         <v>ConVista Schweiz</v>
       </c>
@@ -10889,7 +10845,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="101"/>
+      <c r="A24" s="87"/>
       <c r="B24" s="88"/>
       <c r="C24" s="89"/>
       <c r="D24" s="90" t="str">
@@ -10912,10 +10868,10 @@
         <f aca="false">G24</f>
         <v> </v>
       </c>
-      <c r="J24" s="101" t="n">
+      <c r="J24" s="87" t="n">
         <v>4600</v>
       </c>
-      <c r="K24" s="102" t="str">
+      <c r="K24" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","ConVista USA",IF(ZE!C3="EN","ConVista USA","---"))</f>
         <v>ConVista USA</v>
       </c>
@@ -10937,7 +10893,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="101"/>
+      <c r="A25" s="87"/>
       <c r="B25" s="88"/>
       <c r="C25" s="89"/>
       <c r="D25" s="90" t="str">
@@ -10960,10 +10916,10 @@
         <f aca="false">G25</f>
         <v> </v>
       </c>
-      <c r="J25" s="101" t="n">
+      <c r="J25" s="87" t="n">
         <v>4700</v>
       </c>
-      <c r="K25" s="102" t="str">
+      <c r="K25" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","ConVista GB",IF(ZE!C3="EN","ConVista GB","---"))</f>
         <v>ConVista GB</v>
       </c>
@@ -10985,7 +10941,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="101"/>
+      <c r="A26" s="87"/>
       <c r="B26" s="88"/>
       <c r="C26" s="89"/>
       <c r="D26" s="90" t="str">
@@ -11008,8 +10964,8 @@
         <f aca="false">G26</f>
         <v> </v>
       </c>
-      <c r="J26" s="101"/>
-      <c r="K26" s="103"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="102"/>
       <c r="L26" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J26,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J26,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11028,7 +10984,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="101"/>
+      <c r="A27" s="87"/>
       <c r="B27" s="88"/>
       <c r="C27" s="89"/>
       <c r="D27" s="90" t="str">
@@ -11051,10 +11007,10 @@
         <f aca="false">G27</f>
         <v> </v>
       </c>
-      <c r="J27" s="101" t="n">
+      <c r="J27" s="87" t="n">
         <v>10901</v>
       </c>
-      <c r="K27" s="102" t="str">
+      <c r="K27" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Internes Projekt FS-CD",IF(ZE!C3="EN","Internal Project FS-CD","---"))</f>
         <v>Internes Projekt FS-CD</v>
       </c>
@@ -11076,7 +11032,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="101"/>
+      <c r="A28" s="87"/>
       <c r="B28" s="88"/>
       <c r="C28" s="89"/>
       <c r="D28" s="90" t="str">
@@ -11099,10 +11055,10 @@
         <f aca="false">G28</f>
         <v> </v>
       </c>
-      <c r="J28" s="101" t="n">
+      <c r="J28" s="87" t="n">
         <v>10902</v>
       </c>
-      <c r="K28" s="102" t="str">
+      <c r="K28" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Internes Projekt IS-CS",IF(ZE!C3="EN","Internal Project IS-CS","---"))</f>
         <v>Internes Projekt IS-CS</v>
       </c>
@@ -11124,7 +11080,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="101"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="88"/>
       <c r="C29" s="89"/>
       <c r="D29" s="90" t="str">
@@ -11147,10 +11103,10 @@
         <f aca="false">G29</f>
         <v> </v>
       </c>
-      <c r="J29" s="101" t="n">
+      <c r="J29" s="87" t="n">
         <v>10903</v>
       </c>
-      <c r="K29" s="104" t="str">
+      <c r="K29" s="103" t="str">
         <f aca="false">IF(ZE!C3="DE","Internes Projekt CC-Buch",IF(ZE!C3="EN","Internal Project CC-Buch","---"))</f>
         <v>Internes Projekt CC-Buch</v>
       </c>
@@ -11172,7 +11128,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="101"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="88"/>
       <c r="C30" s="89"/>
       <c r="D30" s="90" t="str">
@@ -11195,10 +11151,10 @@
         <f aca="false">G30</f>
         <v> </v>
       </c>
-      <c r="J30" s="101" t="n">
+      <c r="J30" s="87" t="n">
         <v>10904</v>
       </c>
-      <c r="K30" s="102" t="str">
+      <c r="K30" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Konfig. int. SAP",IF(ZE!C3="EN","Configuration Internal SAP","---"))</f>
         <v>Konfig. int. SAP</v>
       </c>
@@ -11220,7 +11176,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="101"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="88"/>
       <c r="C31" s="89"/>
       <c r="D31" s="90" t="str">
@@ -11243,10 +11199,10 @@
         <f aca="false">G31</f>
         <v> </v>
       </c>
-      <c r="J31" s="101" t="n">
+      <c r="J31" s="87" t="n">
         <v>10905</v>
       </c>
-      <c r="K31" s="102" t="str">
+      <c r="K31" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Internes Projekt CC-Plan",IF(ZE!C3="EN","Internal Project CC-Plan","---"))</f>
         <v>Internes Projekt CC-Plan</v>
       </c>
@@ -11268,7 +11224,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="101"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="88"/>
       <c r="C32" s="89"/>
       <c r="D32" s="90" t="str">
@@ -11291,10 +11247,10 @@
         <f aca="false">G32</f>
         <v> </v>
       </c>
-      <c r="J32" s="101" t="n">
+      <c r="J32" s="87" t="n">
         <v>10906</v>
       </c>
-      <c r="K32" s="102" t="str">
+      <c r="K32" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","AMV (automatisiertes Gerichtl. Mahnverfahren)",IF(ZE!C3="EN","Automatical Judicial Collection Proceeding","---"))</f>
         <v>AMV (automatisiertes Gerichtl. Mahnverfahren)</v>
       </c>
@@ -11316,7 +11272,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="101"/>
+      <c r="A33" s="87"/>
       <c r="B33" s="88"/>
       <c r="C33" s="89"/>
       <c r="D33" s="90" t="str">
@@ -11339,10 +11295,10 @@
         <f aca="false">G33</f>
         <v> </v>
       </c>
-      <c r="J33" s="101" t="n">
+      <c r="J33" s="87" t="n">
         <v>10907</v>
       </c>
-      <c r="K33" s="104" t="str">
+      <c r="K33" s="103" t="str">
         <f aca="false">IF(ZE!C3="DE","CC Test/Internes Projekt Test",IF(ZE!C3="EN","CC Test/Internal Project Test","---"))</f>
         <v>CC Test/Internes Projekt Test</v>
       </c>
@@ -11364,7 +11320,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="101"/>
+      <c r="A34" s="87"/>
       <c r="B34" s="88"/>
       <c r="C34" s="89"/>
       <c r="D34" s="90" t="str">
@@ -11387,8 +11343,8 @@
         <f aca="false">G34</f>
         <v> </v>
       </c>
-      <c r="J34" s="101"/>
-      <c r="K34" s="103"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="102"/>
       <c r="L34" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J34,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J34,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11407,7 +11363,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="101"/>
+      <c r="A35" s="87"/>
       <c r="B35" s="88"/>
       <c r="C35" s="89"/>
       <c r="D35" s="90" t="str">
@@ -11430,10 +11386,10 @@
         <f aca="false">G35</f>
         <v> </v>
       </c>
-      <c r="J35" s="105" t="n">
+      <c r="J35" s="104" t="n">
         <v>99100</v>
       </c>
-      <c r="K35" s="102" t="str">
+      <c r="K35" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Urlaub",IF(ZE!C3="EN","Vacation","---"))</f>
         <v>Urlaub</v>
       </c>
@@ -11455,7 +11411,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="101"/>
+      <c r="A36" s="87"/>
       <c r="B36" s="88"/>
       <c r="C36" s="89"/>
       <c r="D36" s="90" t="str">
@@ -11478,10 +11434,10 @@
         <f aca="false">G36</f>
         <v> </v>
       </c>
-      <c r="J36" s="105" t="n">
+      <c r="J36" s="104" t="n">
         <v>99200</v>
       </c>
-      <c r="K36" s="102" t="str">
+      <c r="K36" s="101" t="str">
         <f aca="false">IF(ZE!C3="DE","Krankheit",IF(ZE!C3="EN","Sickness","---"))</f>
         <v>Krankheit</v>
       </c>
@@ -11503,7 +11459,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="101"/>
+      <c r="A37" s="87"/>
       <c r="B37" s="88"/>
       <c r="C37" s="89"/>
       <c r="D37" s="90" t="str">
@@ -11526,10 +11482,10 @@
         <f aca="false">G37</f>
         <v> </v>
       </c>
-      <c r="J37" s="101" t="n">
+      <c r="J37" s="87" t="n">
         <v>8100</v>
       </c>
-      <c r="K37" s="102" t="s">
+      <c r="K37" s="101" t="s">
         <v>6</v>
       </c>
       <c r="L37" s="96" t="str">
@@ -11550,7 +11506,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="101"/>
+      <c r="A38" s="87"/>
       <c r="B38" s="88"/>
       <c r="C38" s="89"/>
       <c r="D38" s="90" t="str">
@@ -11576,7 +11532,7 @@
       <c r="J38" s="94" t="n">
         <v>2523</v>
       </c>
-      <c r="K38" s="103" t="s">
+      <c r="K38" s="102" t="s">
         <v>7</v>
       </c>
       <c r="L38" s="96" t="str">
@@ -11597,7 +11553,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="101"/>
+      <c r="A39" s="87"/>
       <c r="B39" s="88"/>
       <c r="C39" s="89"/>
       <c r="D39" s="90" t="str">
@@ -11623,7 +11579,7 @@
       <c r="J39" s="46" t="n">
         <v>190028</v>
       </c>
-      <c r="K39" s="103" t="s">
+      <c r="K39" s="102" t="s">
         <v>8</v>
       </c>
       <c r="L39" s="96" t="str">
@@ -11644,7 +11600,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="101"/>
+      <c r="A40" s="87"/>
       <c r="B40" s="88"/>
       <c r="C40" s="89"/>
       <c r="D40" s="90" t="str">
@@ -11667,8 +11623,8 @@
         <f aca="false">G40</f>
         <v> </v>
       </c>
-      <c r="J40" s="101"/>
-      <c r="K40" s="103"/>
+      <c r="J40" s="87"/>
+      <c r="K40" s="102"/>
       <c r="L40" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J40,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J40,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11687,7 +11643,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="101"/>
+      <c r="A41" s="87"/>
       <c r="B41" s="88"/>
       <c r="C41" s="89"/>
       <c r="D41" s="90" t="str">
@@ -11710,10 +11666,10 @@
         <f aca="false">G41</f>
         <v> </v>
       </c>
-      <c r="J41" s="101" t="n">
+      <c r="J41" s="87" t="n">
         <v>672001</v>
       </c>
-      <c r="K41" s="103" t="s">
+      <c r="K41" s="102" t="s">
         <v>9</v>
       </c>
       <c r="L41" s="96" t="n">
@@ -11734,7 +11690,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="101"/>
+      <c r="A42" s="87"/>
       <c r="B42" s="88"/>
       <c r="C42" s="89"/>
       <c r="D42" s="90" t="str">
@@ -11757,8 +11713,8 @@
         <f aca="false">G42</f>
         <v> </v>
       </c>
-      <c r="J42" s="101"/>
-      <c r="K42" s="103"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="102"/>
       <c r="L42" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J42,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J42,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11777,7 +11733,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="101"/>
+      <c r="A43" s="87"/>
       <c r="B43" s="88"/>
       <c r="C43" s="89"/>
       <c r="D43" s="90" t="str">
@@ -11800,8 +11756,8 @@
         <f aca="false">G43</f>
         <v> </v>
       </c>
-      <c r="J43" s="101"/>
-      <c r="K43" s="103"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="102"/>
       <c r="L43" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J43,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J43,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11820,7 +11776,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="101"/>
+      <c r="A44" s="87"/>
       <c r="B44" s="88"/>
       <c r="C44" s="89"/>
       <c r="D44" s="90" t="str">
@@ -11843,8 +11799,8 @@
         <f aca="false">G44</f>
         <v> </v>
       </c>
-      <c r="J44" s="101"/>
-      <c r="K44" s="103"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="102"/>
       <c r="L44" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J44,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J44,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11863,7 +11819,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="101"/>
+      <c r="A45" s="87"/>
       <c r="B45" s="88"/>
       <c r="C45" s="89"/>
       <c r="D45" s="90" t="str">
@@ -11886,8 +11842,8 @@
         <f aca="false">G45</f>
         <v> </v>
       </c>
-      <c r="J45" s="101"/>
-      <c r="K45" s="103"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="102"/>
       <c r="L45" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J45,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J45,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11906,7 +11862,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="101"/>
+      <c r="A46" s="87"/>
       <c r="B46" s="88"/>
       <c r="C46" s="89"/>
       <c r="D46" s="90" t="str">
@@ -11929,8 +11885,8 @@
         <f aca="false">G46</f>
         <v> </v>
       </c>
-      <c r="J46" s="101"/>
-      <c r="K46" s="103"/>
+      <c r="J46" s="87"/>
+      <c r="K46" s="102"/>
       <c r="L46" s="96" t="str">
         <f aca="false">IF(SUMIF(ZE!$H$8:$H$84,J46,ZE!$F$8:$F$84)&lt;&gt;0,SUMIF(ZE!$H$8:$H$84,J46,ZE!$F$8:$F$84)," ")</f>
         <v> </v>
@@ -11949,7 +11905,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="101"/>
+      <c r="A47" s="87"/>
       <c r="B47" s="88"/>
       <c r="C47" s="89"/>
       <c r="D47" s="90" t="str">
@@ -11972,30 +11928,30 @@
         <f aca="false">G47</f>
         <v> </v>
       </c>
-      <c r="J47" s="106" t="str">
+      <c r="J47" s="105" t="str">
         <f aca="false">IF(ZE!C3="DE","Summe interne Kostenstellen",IF(ZE!C3="EN","Total amount for internal cost centres","---"))</f>
         <v>Summe interne Kostenstellen</v>
       </c>
-      <c r="K47" s="107"/>
-      <c r="L47" s="108" t="n">
+      <c r="K47" s="106"/>
+      <c r="L47" s="107" t="n">
         <f aca="false">SUM(L8:L46)</f>
         <v>8.5</v>
       </c>
-      <c r="M47" s="109" t="n">
+      <c r="M47" s="108" t="n">
         <f aca="false">SUM(M8:M46)</f>
         <v>1.0625</v>
       </c>
-      <c r="N47" s="110" t="n">
+      <c r="N47" s="109" t="n">
         <f aca="false">SUM(N8:N46)</f>
         <v>0</v>
       </c>
-      <c r="O47" s="110" t="n">
+      <c r="O47" s="109" t="n">
         <f aca="false">SUM(O8:O46)</f>
         <v>1.0625</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="101"/>
+      <c r="A48" s="87"/>
       <c r="B48" s="88"/>
       <c r="C48" s="89"/>
       <c r="D48" s="90" t="str">
@@ -12018,15 +11974,15 @@
         <f aca="false">G48</f>
         <v> </v>
       </c>
-      <c r="J48" s="111"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="111"/>
-      <c r="M48" s="111"/>
-      <c r="N48" s="111"/>
-      <c r="O48" s="111"/>
+      <c r="J48" s="110"/>
+      <c r="K48" s="111"/>
+      <c r="L48" s="110"/>
+      <c r="M48" s="110"/>
+      <c r="N48" s="110"/>
+      <c r="O48" s="110"/>
     </row>
     <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="101"/>
+      <c r="A49" s="87"/>
       <c r="B49" s="88"/>
       <c r="C49" s="89"/>
       <c r="D49" s="90" t="str">
@@ -12049,15 +12005,15 @@
         <f aca="false">G49</f>
         <v> </v>
       </c>
-      <c r="J49" s="111"/>
-      <c r="K49" s="112"/>
-      <c r="L49" s="111"/>
-      <c r="M49" s="111"/>
-      <c r="N49" s="111"/>
-      <c r="O49" s="111"/>
+      <c r="J49" s="110"/>
+      <c r="K49" s="111"/>
+      <c r="L49" s="110"/>
+      <c r="M49" s="110"/>
+      <c r="N49" s="110"/>
+      <c r="O49" s="110"/>
     </row>
     <row r="50" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="101"/>
+      <c r="A50" s="87"/>
       <c r="B50" s="88"/>
       <c r="C50" s="89"/>
       <c r="D50" s="90" t="str">
@@ -12088,7 +12044,7 @@
       <c r="O50" s="75"/>
     </row>
     <row r="51" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="101"/>
+      <c r="A51" s="87"/>
       <c r="B51" s="88"/>
       <c r="C51" s="89"/>
       <c r="D51" s="90" t="str">
@@ -12134,7 +12090,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="101"/>
+      <c r="A52" s="87"/>
       <c r="B52" s="88"/>
       <c r="C52" s="89"/>
       <c r="D52" s="90" t="str">
@@ -12157,7 +12113,7 @@
         <f aca="false">G52</f>
         <v> </v>
       </c>
-      <c r="J52" s="113" t="str">
+      <c r="J52" s="112" t="str">
         <f aca="false">IF(ZE!C3="DE","Bezeichnung",IF(ZE!C3="EN","Description","---"))</f>
         <v>Bezeichnung</v>
       </c>
@@ -12180,7 +12136,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="101"/>
+      <c r="A53" s="87"/>
       <c r="B53" s="88"/>
       <c r="C53" s="89"/>
       <c r="D53" s="90" t="str">
@@ -12203,7 +12159,7 @@
         <f aca="false">G53</f>
         <v> </v>
       </c>
-      <c r="J53" s="114"/>
+      <c r="J53" s="113"/>
       <c r="K53" s="86"/>
       <c r="L53" s="39"/>
       <c r="M53" s="38"/>
@@ -12211,7 +12167,7 @@
       <c r="O53" s="75"/>
     </row>
     <row r="54" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="101"/>
+      <c r="A54" s="87"/>
       <c r="B54" s="88"/>
       <c r="C54" s="89"/>
       <c r="D54" s="90" t="str">
@@ -12234,30 +12190,30 @@
         <f aca="false">G54</f>
         <v> </v>
       </c>
-      <c r="J54" s="115" t="str">
+      <c r="J54" s="114" t="str">
         <f aca="false">IF(ZE!C3="DE","Externe Kostenstellen",IF(ZE!C3="EN","External cost centres","---"))</f>
         <v>Externe Kostenstellen</v>
       </c>
-      <c r="K54" s="116"/>
-      <c r="L54" s="117" t="n">
+      <c r="K54" s="115"/>
+      <c r="L54" s="116" t="n">
         <f aca="false">E61</f>
         <v>0</v>
       </c>
-      <c r="M54" s="118" t="n">
+      <c r="M54" s="117" t="n">
         <f aca="false">G61</f>
         <v>0</v>
       </c>
-      <c r="N54" s="119" t="n">
+      <c r="N54" s="118" t="n">
         <f aca="false">F61</f>
         <v>0</v>
       </c>
-      <c r="O54" s="120" t="n">
+      <c r="O54" s="119" t="n">
         <f aca="false">H61</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="101"/>
+      <c r="A55" s="87"/>
       <c r="B55" s="88"/>
       <c r="C55" s="89"/>
       <c r="D55" s="90" t="str">
@@ -12280,29 +12236,29 @@
         <f aca="false">G55</f>
         <v> </v>
       </c>
-      <c r="J55" s="121" t="str">
+      <c r="J55" s="120" t="str">
         <f aca="false">IF(ZE!C3="DE","Interne Kostenstellen",IF(ZE!C3="EN","Internal cost centres","---"))</f>
         <v>Interne Kostenstellen</v>
       </c>
-      <c r="K55" s="122"/>
+      <c r="K55" s="121"/>
       <c r="L55" s="99" t="n">
         <f aca="false">M47</f>
         <v>1.0625</v>
       </c>
-      <c r="M55" s="123" t="s">
+      <c r="M55" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="N55" s="124" t="n">
+      <c r="N55" s="123" t="n">
         <f aca="false">N47</f>
         <v>0</v>
       </c>
-      <c r="O55" s="125" t="n">
+      <c r="O55" s="124" t="n">
         <f aca="false">O47</f>
         <v>1.0625</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="101"/>
+      <c r="A56" s="87"/>
       <c r="B56" s="88"/>
       <c r="C56" s="89"/>
       <c r="D56" s="90" t="str">
@@ -12325,27 +12281,27 @@
         <f aca="false">G56</f>
         <v> </v>
       </c>
-      <c r="J56" s="126" t="str">
+      <c r="J56" s="125" t="str">
         <f aca="false">IF(ZE!C3="DE","Reisezeiten-Übertrag (50%)",IF(ZE!C3="EN","Travel time transfer (50%)","---"))</f>
         <v>Reisezeiten-Übertrag (50%)</v>
       </c>
-      <c r="K56" s="127"/>
-      <c r="L56" s="128" t="s">
+      <c r="K56" s="126"/>
+      <c r="L56" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="M56" s="128" t="s">
+      <c r="M56" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="N56" s="128" t="s">
+      <c r="N56" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="O56" s="129" t="n">
+      <c r="O56" s="128" t="n">
         <f aca="false">(N54+N55)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="101"/>
+      <c r="A57" s="87"/>
       <c r="B57" s="88"/>
       <c r="C57" s="89"/>
       <c r="D57" s="90" t="str">
@@ -12368,30 +12324,30 @@
         <f aca="false">G57</f>
         <v> </v>
       </c>
-      <c r="J57" s="130" t="str">
+      <c r="J57" s="129" t="str">
         <f aca="false">IF(ZE!C3="DE","Summe alle Kostenstellen",IF(ZE!C3="EN","Total amount for all cost centres","---"))</f>
         <v>Summe alle Kostenstellen</v>
       </c>
-      <c r="K57" s="131"/>
-      <c r="L57" s="132" t="n">
+      <c r="K57" s="130"/>
+      <c r="L57" s="131" t="n">
         <f aca="false">SUM(L54:L55)</f>
         <v>1.0625</v>
       </c>
-      <c r="M57" s="132" t="n">
+      <c r="M57" s="131" t="n">
         <f aca="false">SUM(M54:M55)</f>
         <v>0</v>
       </c>
-      <c r="N57" s="132" t="n">
+      <c r="N57" s="131" t="n">
         <f aca="false">SUM(N54:N55)</f>
         <v>0</v>
       </c>
-      <c r="O57" s="133" t="n">
+      <c r="O57" s="132" t="n">
         <f aca="false">SUM(O54:O56)</f>
         <v>1.0625</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="101"/>
+      <c r="A58" s="87"/>
       <c r="B58" s="88"/>
       <c r="C58" s="89"/>
       <c r="D58" s="90" t="str">
@@ -12414,28 +12370,28 @@
         <f aca="false">G58</f>
         <v> </v>
       </c>
-      <c r="J58" s="134" t="str">
+      <c r="J58" s="133" t="str">
         <f aca="false">IF(ZE!C3="DE","Urlaub",IF(ZE!C3="EN","Vacation","---"))</f>
         <v>Urlaub</v>
       </c>
-      <c r="K58" s="135"/>
-      <c r="L58" s="136" t="n">
+      <c r="K58" s="134"/>
+      <c r="L58" s="135" t="n">
         <f aca="false">IF(M35=" ",0,M35)</f>
         <v>0</v>
       </c>
-      <c r="M58" s="128" t="s">
+      <c r="M58" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="N58" s="128" t="s">
+      <c r="N58" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="O58" s="129" t="n">
+      <c r="O58" s="128" t="n">
         <f aca="false">L58</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="101"/>
+      <c r="A59" s="87"/>
       <c r="B59" s="88"/>
       <c r="C59" s="89"/>
       <c r="D59" s="90" t="str">
@@ -12458,28 +12414,28 @@
         <f aca="false">G59</f>
         <v> </v>
       </c>
-      <c r="J59" s="134" t="str">
+      <c r="J59" s="133" t="str">
         <f aca="false">IF(ZE!C3="DE","Krankheit",IF(ZE!C3="EN","Sickness","---"))</f>
         <v>Krankheit</v>
       </c>
-      <c r="K59" s="135"/>
-      <c r="L59" s="136" t="n">
+      <c r="K59" s="134"/>
+      <c r="L59" s="135" t="n">
         <f aca="false">IF(M36=" ",0,M36)</f>
         <v>0</v>
       </c>
-      <c r="M59" s="128" t="s">
+      <c r="M59" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="N59" s="128" t="s">
+      <c r="N59" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="O59" s="129" t="n">
+      <c r="O59" s="128" t="n">
         <f aca="false">L59</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="101"/>
+      <c r="A60" s="87"/>
       <c r="B60" s="88"/>
       <c r="C60" s="89"/>
       <c r="D60" s="90" t="str">
@@ -12502,68 +12458,68 @@
         <f aca="false">G60</f>
         <v> </v>
       </c>
-      <c r="J60" s="137" t="str">
+      <c r="J60" s="136" t="str">
         <f aca="false">IF(ZE!C3="DE","Sollarbeitstage",IF(ZE!C3="EN","Total working days for the month","---"))</f>
         <v>Sollarbeitstage</v>
       </c>
-      <c r="K60" s="138"/>
-      <c r="L60" s="139" t="n">
+      <c r="K60" s="137"/>
+      <c r="L60" s="138" t="n">
         <v>0</v>
       </c>
-      <c r="M60" s="140" t="s">
+      <c r="M60" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="N60" s="141" t="s">
+      <c r="N60" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O60" s="133" t="n">
+      <c r="O60" s="132" t="n">
         <f aca="false">L60</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="106" t="str">
+      <c r="A61" s="105" t="str">
         <f aca="false">IF(ZE!C3="DE","Summe externe Kostenstellen",IF(ZE!C3="EN","Total amount for internal cost centres","---"))</f>
         <v>Summe externe Kostenstellen</v>
       </c>
-      <c r="B61" s="131"/>
-      <c r="C61" s="142"/>
-      <c r="D61" s="143" t="n">
+      <c r="B61" s="130"/>
+      <c r="C61" s="141"/>
+      <c r="D61" s="142" t="n">
         <f aca="false">SUM(D8:D60)</f>
         <v>0</v>
       </c>
-      <c r="E61" s="144" t="n">
+      <c r="E61" s="143" t="n">
         <f aca="false">SUM(E8:E60)</f>
         <v>0</v>
       </c>
-      <c r="F61" s="144" t="n">
+      <c r="F61" s="143" t="n">
         <f aca="false">SUM(F8:F60)</f>
         <v>0</v>
       </c>
-      <c r="G61" s="144" t="n">
+      <c r="G61" s="143" t="n">
         <f aca="false">SUM(G8:G60)</f>
         <v>0</v>
       </c>
-      <c r="H61" s="144" t="n">
+      <c r="H61" s="143" t="n">
         <f aca="false">SUM(H8:H60)</f>
         <v>0</v>
       </c>
-      <c r="J61" s="145" t="str">
+      <c r="J61" s="144" t="str">
         <f aca="false">IF(ZE!C3="DE","Gesamtsumme",IF(ZE!C3="EN","Work account status","---"))</f>
         <v>Gesamtsumme</v>
       </c>
-      <c r="K61" s="146"/>
-      <c r="L61" s="147" t="n">
+      <c r="K61" s="145"/>
+      <c r="L61" s="146" t="n">
         <f aca="false">L57-L60</f>
         <v>1.0625</v>
       </c>
-      <c r="M61" s="148" t="s">
+      <c r="M61" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="N61" s="149" t="s">
+      <c r="N61" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="O61" s="150" t="n">
+      <c r="O61" s="149" t="n">
         <f aca="false">O57-O60</f>
         <v>1.0625</v>
       </c>
@@ -12622,56 +12578,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="151" width="12.015306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="151" width="43.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="151" width="9.69897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="150" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="150" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="150" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="152" t="str">
+      <c r="A1" s="151" t="str">
         <f aca="false">IF(ZE!C3="DE","Planzahlen",IF(ZE!C3="EN","Work Schedule","---"))</f>
         <v>Planzahlen</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="153" t="str">
+      <c r="B1" s="151"/>
+      <c r="C1" s="152" t="str">
         <f aca="false">ZE!E1</f>
         <v>Januar</v>
       </c>
-      <c r="D1" s="154" t="n">
+      <c r="D1" s="153" t="n">
         <f aca="false">ZE!H1</f>
-        <v>2018</v>
-      </c>
-      <c r="E1" s="152"/>
-      <c r="F1" s="155"/>
+        <v>2019</v>
+      </c>
+      <c r="E1" s="151"/>
+      <c r="F1" s="154"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="156" t="str">
+      <c r="A2" s="155" t="str">
         <f aca="false">ZE!A2</f>
         <v>Gerald Kahrer</v>
       </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="156" t="str">
+      <c r="B2" s="156"/>
+      <c r="C2" s="155" t="str">
         <f aca="false">ZE!G2</f>
         <v>Pers-Nr.:</v>
       </c>
-      <c r="D2" s="156"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="159"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="158"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="160"/>
-      <c r="B3" s="159"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
+      <c r="A3" s="159"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17"/>
       <c r="B4" s="20"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="162"/>
+      <c r="E4" s="161"/>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="79" t="str">
@@ -12679,12 +12635,12 @@
         <v>Kostenstelle</v>
       </c>
       <c r="B5" s="79"/>
-      <c r="C5" s="163" t="str">
+      <c r="C5" s="162" t="str">
         <f aca="false">IF(ZE!C3="DE","Planzahlen in Tagen",IF(ZE!C3="EN","Work Schedule in days","---"))</f>
         <v>Planzahlen in Tagen</v>
       </c>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="80" t="str">
@@ -12695,606 +12651,606 @@
         <f aca="false">IF(ZE!C3="DE","Kst-Bezeichnung",IF(ZE!C3="EN","Description","---"))</f>
         <v>Kst-Bezeichnung</v>
       </c>
-      <c r="C6" s="164" t="n">
+      <c r="C6" s="163" t="n">
         <f aca="false">IF(MOD(ZE!H3+1,12)=0,12,MOD(ZE!H3+1,12))</f>
         <v>2</v>
       </c>
-      <c r="D6" s="164" t="n">
+      <c r="D6" s="163" t="n">
         <f aca="false">IF(MOD(ZE!H3+2,12)=0,12,MOD(ZE!H3+2,12))</f>
         <v>3</v>
       </c>
-      <c r="E6" s="165" t="n">
+      <c r="E6" s="164" t="n">
         <f aca="false">IF(MOD(ZE!H3+3,12)=0,12,MOD(ZE!H3+3,12))</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="166"/>
-      <c r="B7" s="167"/>
-      <c r="C7" s="168"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="170"/>
+      <c r="A7" s="165"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="168"/>
+      <c r="E7" s="169"/>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="171" t="str">
+      <c r="A8" s="170" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A8 = " ",'ZE-Sum'!A8 = 0), " ", 'ZE-Sum'!A8)</f>
         <v> </v>
       </c>
-      <c r="B8" s="172" t="e">
+      <c r="B8" s="171" t="e">
         <f aca="false">IF(OR(A8=0,A8= " ")," ",IF(ISERROR(VLOOKUP(A8,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A8,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A8,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A8,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C8" s="173" t="n">
+      <c r="C8" s="172" t="n">
         <v>15</v>
       </c>
-      <c r="D8" s="174" t="n">
+      <c r="D8" s="173" t="n">
         <v>20</v>
       </c>
-      <c r="E8" s="175" t="n">
+      <c r="E8" s="174" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="176" t="str">
+      <c r="A9" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A9 = " ",'ZE-Sum'!A9 = 0), " ", 'ZE-Sum'!A9)</f>
         <v> </v>
       </c>
-      <c r="B9" s="177" t="e">
+      <c r="B9" s="176" t="e">
         <f aca="false">IF(OR(A9=0,A9= " ")," ",IF(ISERROR(VLOOKUP(A9,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A9,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A9,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A9,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C9" s="178"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="180"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="179"/>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="176" t="str">
+      <c r="A10" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A10 = " ",'ZE-Sum'!A10 = 0), " ", 'ZE-Sum'!A10)</f>
         <v> </v>
       </c>
-      <c r="B10" s="177" t="e">
+      <c r="B10" s="176" t="e">
         <f aca="false">IF(OR(A10=0,A10= " ")," ",IF(ISERROR(VLOOKUP(A10,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A10,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A10,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A10,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C10" s="178"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="180"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="178"/>
+      <c r="E10" s="179"/>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="176" t="str">
+      <c r="A11" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A11 = " ",'ZE-Sum'!A11 = 0), " ", 'ZE-Sum'!A11)</f>
         <v> </v>
       </c>
-      <c r="B11" s="177" t="e">
+      <c r="B11" s="176" t="e">
         <f aca="false">IF(OR(A11=0,A11= " ")," ",IF(ISERROR(VLOOKUP(A11,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A11,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A11,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A11,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C11" s="178"/>
-      <c r="D11" s="179"/>
-      <c r="E11" s="180"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="179"/>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="176" t="str">
+      <c r="A12" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A12 = " ",'ZE-Sum'!A12 = 0), " ", 'ZE-Sum'!A12)</f>
         <v> </v>
       </c>
-      <c r="B12" s="177" t="e">
+      <c r="B12" s="176" t="e">
         <f aca="false">IF(OR(A12=0,A12= " ")," ",IF(ISERROR(VLOOKUP(A12,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A12,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A12,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A12,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C12" s="178"/>
-      <c r="D12" s="179"/>
-      <c r="E12" s="180"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="176" t="str">
+      <c r="A13" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A13 = " ",'ZE-Sum'!A13 = 0), " ", 'ZE-Sum'!A13)</f>
         <v> </v>
       </c>
-      <c r="B13" s="177" t="e">
+      <c r="B13" s="176" t="e">
         <f aca="false">IF(OR(A13=0,A13= " ")," ",IF(ISERROR(VLOOKUP(A13,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A13,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A13,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A13,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C13" s="178"/>
-      <c r="D13" s="179"/>
-      <c r="E13" s="180"/>
+      <c r="C13" s="177"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="179"/>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="176" t="str">
+      <c r="A14" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A14 = " ",'ZE-Sum'!A14 = 0), " ", 'ZE-Sum'!A14)</f>
         <v> </v>
       </c>
-      <c r="B14" s="177" t="e">
+      <c r="B14" s="176" t="e">
         <f aca="false">IF(OR(A14=0,A14= " ")," ",IF(ISERROR(VLOOKUP(A14,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A14,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A14,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A14,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C14" s="178"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="C14" s="177"/>
+      <c r="D14" s="178"/>
+      <c r="E14" s="179"/>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="176" t="str">
+      <c r="A15" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A15 = " ",'ZE-Sum'!A15 = 0), " ", 'ZE-Sum'!A15)</f>
         <v> </v>
       </c>
-      <c r="B15" s="177" t="e">
+      <c r="B15" s="176" t="e">
         <f aca="false">IF(OR(A15=0,A15= " ")," ",IF(ISERROR(VLOOKUP(A15,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A15,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A15,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A15,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C15" s="178"/>
-      <c r="D15" s="179"/>
-      <c r="E15" s="180"/>
+      <c r="C15" s="177"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="179"/>
     </row>
     <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="176" t="str">
+      <c r="A16" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A16 = " ",'ZE-Sum'!A16 = 0), " ", 'ZE-Sum'!A16)</f>
         <v> </v>
       </c>
-      <c r="B16" s="177" t="e">
+      <c r="B16" s="176" t="e">
         <f aca="false">IF(OR(A16=0,A16= " ")," ",IF(ISERROR(VLOOKUP(A16,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A16,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A16,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A16,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C16" s="178"/>
-      <c r="D16" s="179"/>
-      <c r="E16" s="180"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="179"/>
     </row>
     <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="176" t="str">
+      <c r="A17" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A17 = " ",'ZE-Sum'!A17 = 0), " ", 'ZE-Sum'!A17)</f>
         <v> </v>
       </c>
-      <c r="B17" s="177" t="e">
+      <c r="B17" s="176" t="e">
         <f aca="false">IF(OR(A17=0,A17= " ")," ",IF(ISERROR(VLOOKUP(A17,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A17,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A17,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A17,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C17" s="178"/>
-      <c r="D17" s="179"/>
-      <c r="E17" s="180"/>
+      <c r="C17" s="177"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="179"/>
     </row>
     <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="176" t="str">
+      <c r="A18" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A18 = " ",'ZE-Sum'!A18 = 0), " ", 'ZE-Sum'!A18)</f>
         <v> </v>
       </c>
-      <c r="B18" s="177" t="e">
+      <c r="B18" s="176" t="e">
         <f aca="false">IF(OR(A18=0,A18= " ")," ",IF(ISERROR(VLOOKUP(A18,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A18,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A18,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A18,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C18" s="178"/>
-      <c r="D18" s="179"/>
-      <c r="E18" s="180"/>
+      <c r="C18" s="177"/>
+      <c r="D18" s="178"/>
+      <c r="E18" s="179"/>
     </row>
     <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="176" t="str">
+      <c r="A19" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A19 = " ",'ZE-Sum'!A19 = 0), " ", 'ZE-Sum'!A19)</f>
         <v> </v>
       </c>
-      <c r="B19" s="177" t="e">
+      <c r="B19" s="176" t="e">
         <f aca="false">IF(OR(A19=0,A19= " ")," ",IF(ISERROR(VLOOKUP(A19,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A19,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A19,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A19,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C19" s="178"/>
-      <c r="D19" s="179"/>
-      <c r="E19" s="180"/>
+      <c r="C19" s="177"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="179"/>
     </row>
     <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="176" t="str">
+      <c r="A20" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A20 = " ",'ZE-Sum'!A20 = 0), " ", 'ZE-Sum'!A20)</f>
         <v> </v>
       </c>
-      <c r="B20" s="177" t="e">
+      <c r="B20" s="176" t="e">
         <f aca="false">IF(OR(A20=0,A20= " ")," ",IF(ISERROR(VLOOKUP(A20,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A20,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A20,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A20,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C20" s="178"/>
-      <c r="D20" s="179"/>
-      <c r="E20" s="180"/>
+      <c r="C20" s="177"/>
+      <c r="D20" s="178"/>
+      <c r="E20" s="179"/>
     </row>
     <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="176" t="str">
+      <c r="A21" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A21 = " ",'ZE-Sum'!A21 = 0), " ", 'ZE-Sum'!A21)</f>
         <v> </v>
       </c>
-      <c r="B21" s="177" t="e">
+      <c r="B21" s="176" t="e">
         <f aca="false">IF(OR(A21=0,A21= " ")," ",IF(ISERROR(VLOOKUP(A21,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A21,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A21,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A21,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C21" s="178"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="180"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="176" t="str">
+      <c r="A22" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A22 = " ",'ZE-Sum'!A22 = 0), " ", 'ZE-Sum'!A22)</f>
         <v> </v>
       </c>
-      <c r="B22" s="177" t="e">
+      <c r="B22" s="176" t="e">
         <f aca="false">IF(OR(A22=0,A22= " ")," ",IF(ISERROR(VLOOKUP(A22,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A22,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A22,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A22,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C22" s="178"/>
-      <c r="D22" s="179"/>
-      <c r="E22" s="180"/>
+      <c r="C22" s="177"/>
+      <c r="D22" s="178"/>
+      <c r="E22" s="179"/>
     </row>
     <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="176" t="str">
+      <c r="A23" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A23 = " ",'ZE-Sum'!A23 = 0), " ", 'ZE-Sum'!A23)</f>
         <v> </v>
       </c>
-      <c r="B23" s="177" t="e">
+      <c r="B23" s="176" t="e">
         <f aca="false">IF(OR(A23=0,A23= " ")," ",IF(ISERROR(VLOOKUP(A23,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A23,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A23,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A23,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C23" s="178"/>
-      <c r="D23" s="179"/>
-      <c r="E23" s="180"/>
+      <c r="C23" s="177"/>
+      <c r="D23" s="178"/>
+      <c r="E23" s="179"/>
     </row>
     <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="176" t="str">
+      <c r="A24" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A24 = " ",'ZE-Sum'!A24 = 0), " ", 'ZE-Sum'!A24)</f>
         <v> </v>
       </c>
-      <c r="B24" s="177" t="e">
+      <c r="B24" s="176" t="e">
         <f aca="false">IF(OR(A24=0,A24= " ")," ",IF(ISERROR(VLOOKUP(A24,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A24,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A24,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A24,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C24" s="178"/>
-      <c r="D24" s="179"/>
-      <c r="E24" s="180"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="178"/>
+      <c r="E24" s="179"/>
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="176" t="str">
+      <c r="A25" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A25 = " ",'ZE-Sum'!A25 = 0), " ", 'ZE-Sum'!A25)</f>
         <v> </v>
       </c>
-      <c r="B25" s="177" t="e">
+      <c r="B25" s="176" t="e">
         <f aca="false">IF(OR(A25=0,A25= " ")," ",IF(ISERROR(VLOOKUP(A25,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A25,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A25,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A25,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C25" s="178"/>
-      <c r="D25" s="179"/>
-      <c r="E25" s="180"/>
+      <c r="C25" s="177"/>
+      <c r="D25" s="178"/>
+      <c r="E25" s="179"/>
     </row>
     <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="176" t="str">
+      <c r="A26" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A26 = " ",'ZE-Sum'!A26 = 0), " ", 'ZE-Sum'!A26)</f>
         <v> </v>
       </c>
-      <c r="B26" s="177" t="e">
+      <c r="B26" s="176" t="e">
         <f aca="false">IF(OR(A26=0,A26= " ")," ",IF(ISERROR(VLOOKUP(A26,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A26,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A26,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A26,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C26" s="178"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="180"/>
+      <c r="C26" s="177"/>
+      <c r="D26" s="178"/>
+      <c r="E26" s="179"/>
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="176" t="str">
+      <c r="A27" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A27 = " ",'ZE-Sum'!A27 = 0), " ", 'ZE-Sum'!A27)</f>
         <v> </v>
       </c>
-      <c r="B27" s="177" t="e">
+      <c r="B27" s="176" t="e">
         <f aca="false">IF(OR(A27=0,A27= " ")," ",IF(ISERROR(VLOOKUP(A27,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A27,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A27,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A27,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C27" s="178"/>
-      <c r="D27" s="179"/>
-      <c r="E27" s="180"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="178"/>
+      <c r="E27" s="179"/>
     </row>
     <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="176" t="str">
+      <c r="A28" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A28 = " ",'ZE-Sum'!A28 = 0), " ", 'ZE-Sum'!A28)</f>
         <v> </v>
       </c>
-      <c r="B28" s="177" t="e">
+      <c r="B28" s="176" t="e">
         <f aca="false">IF(OR(A28=0,A28= " ")," ",IF(ISERROR(VLOOKUP(A28,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A28,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A28,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A28,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C28" s="178"/>
-      <c r="D28" s="179"/>
-      <c r="E28" s="180"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="178"/>
+      <c r="E28" s="179"/>
     </row>
     <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="176" t="str">
+      <c r="A29" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A29 = " ",'ZE-Sum'!A29 = 0), " ", 'ZE-Sum'!A29)</f>
         <v> </v>
       </c>
-      <c r="B29" s="177" t="e">
+      <c r="B29" s="176" t="e">
         <f aca="false">IF(OR(A29=0,A29= " ")," ",IF(ISERROR(VLOOKUP(A29,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A29,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A29,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A29,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C29" s="178"/>
-      <c r="D29" s="179"/>
-      <c r="E29" s="180"/>
+      <c r="C29" s="177"/>
+      <c r="D29" s="178"/>
+      <c r="E29" s="179"/>
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="176" t="str">
+      <c r="A30" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A30 = " ",'ZE-Sum'!A30 = 0), " ", 'ZE-Sum'!A30)</f>
         <v> </v>
       </c>
-      <c r="B30" s="177" t="e">
+      <c r="B30" s="176" t="e">
         <f aca="false">IF(OR(A30=0,A30= " ")," ",IF(ISERROR(VLOOKUP(A30,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A30,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A30,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A30,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C30" s="178"/>
-      <c r="D30" s="179"/>
-      <c r="E30" s="180"/>
+      <c r="C30" s="177"/>
+      <c r="D30" s="178"/>
+      <c r="E30" s="179"/>
     </row>
     <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="176" t="str">
+      <c r="A31" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A31 = " ",'ZE-Sum'!A31 = 0), " ", 'ZE-Sum'!A31)</f>
         <v> </v>
       </c>
-      <c r="B31" s="177" t="e">
+      <c r="B31" s="176" t="e">
         <f aca="false">IF(OR(A31=0,A31= " ")," ",IF(ISERROR(VLOOKUP(A31,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A31,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A31,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A31,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C31" s="178"/>
-      <c r="D31" s="179"/>
-      <c r="E31" s="180"/>
+      <c r="C31" s="177"/>
+      <c r="D31" s="178"/>
+      <c r="E31" s="179"/>
     </row>
     <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="176" t="str">
+      <c r="A32" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A32 = " ",'ZE-Sum'!A32 = 0), " ", 'ZE-Sum'!A32)</f>
         <v> </v>
       </c>
-      <c r="B32" s="177" t="e">
+      <c r="B32" s="176" t="e">
         <f aca="false">IF(OR(A32=0,A32= " ")," ",IF(ISERROR(VLOOKUP(A32,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A32,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A32,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A32,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C32" s="178"/>
-      <c r="D32" s="179"/>
-      <c r="E32" s="180"/>
+      <c r="C32" s="177"/>
+      <c r="D32" s="178"/>
+      <c r="E32" s="179"/>
     </row>
     <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="176" t="str">
+      <c r="A33" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A33 = " ",'ZE-Sum'!A33 = 0), " ", 'ZE-Sum'!A33)</f>
         <v> </v>
       </c>
-      <c r="B33" s="177" t="e">
+      <c r="B33" s="176" t="e">
         <f aca="false">IF(OR(A33=0,A33= " ")," ",IF(ISERROR(VLOOKUP(A33,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A33,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A33,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A33,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C33" s="178"/>
-      <c r="D33" s="179"/>
-      <c r="E33" s="180"/>
+      <c r="C33" s="177"/>
+      <c r="D33" s="178"/>
+      <c r="E33" s="179"/>
     </row>
     <row r="34" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="176" t="str">
+      <c r="A34" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A34 = " ",'ZE-Sum'!A34 = 0), " ", 'ZE-Sum'!A34)</f>
         <v> </v>
       </c>
-      <c r="B34" s="177" t="e">
+      <c r="B34" s="176" t="e">
         <f aca="false">IF(OR(A34=0,A34= " ")," ",IF(ISERROR(VLOOKUP(A34,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A34,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A34,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A34,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C34" s="178"/>
-      <c r="D34" s="179"/>
-      <c r="E34" s="180"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="178"/>
+      <c r="E34" s="179"/>
     </row>
     <row r="35" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="176" t="str">
+      <c r="A35" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A35 = " ",'ZE-Sum'!A35 = 0), " ", 'ZE-Sum'!A35)</f>
         <v> </v>
       </c>
-      <c r="B35" s="177" t="e">
+      <c r="B35" s="176" t="e">
         <f aca="false">IF(OR(A35=0,A35= " ")," ",IF(ISERROR(VLOOKUP(A35,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A35,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A35,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A35,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C35" s="178"/>
-      <c r="D35" s="179"/>
-      <c r="E35" s="180"/>
+      <c r="C35" s="177"/>
+      <c r="D35" s="178"/>
+      <c r="E35" s="179"/>
     </row>
     <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="176" t="str">
+      <c r="A36" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A36 = " ",'ZE-Sum'!A36 = 0), " ", 'ZE-Sum'!A36)</f>
         <v> </v>
       </c>
-      <c r="B36" s="177" t="e">
+      <c r="B36" s="176" t="e">
         <f aca="false">IF(OR(A36=0,A36= " ")," ",IF(ISERROR(VLOOKUP(A36,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A36,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A36,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A36,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C36" s="178"/>
-      <c r="D36" s="179"/>
-      <c r="E36" s="180"/>
+      <c r="C36" s="177"/>
+      <c r="D36" s="178"/>
+      <c r="E36" s="179"/>
     </row>
     <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="176" t="str">
+      <c r="A37" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A37 = " ",'ZE-Sum'!A37 = 0), " ", 'ZE-Sum'!A37)</f>
         <v> </v>
       </c>
-      <c r="B37" s="177" t="e">
+      <c r="B37" s="176" t="e">
         <f aca="false">IF(OR(A37=0,A37= " ")," ",IF(ISERROR(VLOOKUP(A37,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A37,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A37,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A37,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C37" s="178"/>
-      <c r="D37" s="179"/>
-      <c r="E37" s="180"/>
+      <c r="C37" s="177"/>
+      <c r="D37" s="178"/>
+      <c r="E37" s="179"/>
     </row>
     <row r="38" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="176" t="str">
+      <c r="A38" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A38 = " ",'ZE-Sum'!A38 = 0), " ", 'ZE-Sum'!A38)</f>
         <v> </v>
       </c>
-      <c r="B38" s="177" t="e">
+      <c r="B38" s="176" t="e">
         <f aca="false">IF(OR(A38=0,A38= " ")," ",IF(ISERROR(VLOOKUP(A38,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A38,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A38,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A38,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C38" s="178"/>
-      <c r="D38" s="179"/>
-      <c r="E38" s="180"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="178"/>
+      <c r="E38" s="179"/>
     </row>
     <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="176" t="str">
+      <c r="A39" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A39 = " ",'ZE-Sum'!A39 = 0), " ", 'ZE-Sum'!A39)</f>
         <v> </v>
       </c>
-      <c r="B39" s="177" t="e">
+      <c r="B39" s="176" t="e">
         <f aca="false">IF(OR(A39=0,A39= " ")," ",IF(ISERROR(VLOOKUP(A39,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A39,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A39,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A39,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C39" s="178"/>
-      <c r="D39" s="179"/>
-      <c r="E39" s="180"/>
+      <c r="C39" s="177"/>
+      <c r="D39" s="178"/>
+      <c r="E39" s="179"/>
     </row>
     <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="176" t="str">
+      <c r="A40" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A40 = " ",'ZE-Sum'!A40 = 0), " ", 'ZE-Sum'!A40)</f>
         <v> </v>
       </c>
-      <c r="B40" s="177" t="e">
+      <c r="B40" s="176" t="e">
         <f aca="false">IF(OR(A40=0,A40= " ")," ",IF(ISERROR(VLOOKUP(A40,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A40,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A40,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A40,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C40" s="178"/>
-      <c r="D40" s="179"/>
-      <c r="E40" s="180"/>
+      <c r="C40" s="177"/>
+      <c r="D40" s="178"/>
+      <c r="E40" s="179"/>
     </row>
     <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="176" t="str">
+      <c r="A41" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A41 = " ",'ZE-Sum'!A41 = 0), " ", 'ZE-Sum'!A41)</f>
         <v> </v>
       </c>
-      <c r="B41" s="177" t="e">
+      <c r="B41" s="176" t="e">
         <f aca="false">IF(OR(A41=0,A41= " ")," ",IF(ISERROR(VLOOKUP(A41,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A41,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A41,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A41,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C41" s="178"/>
-      <c r="D41" s="179"/>
-      <c r="E41" s="180"/>
+      <c r="C41" s="177"/>
+      <c r="D41" s="178"/>
+      <c r="E41" s="179"/>
     </row>
     <row r="42" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="176" t="str">
+      <c r="A42" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A42 = " ",'ZE-Sum'!A42 = 0), " ", 'ZE-Sum'!A42)</f>
         <v> </v>
       </c>
-      <c r="B42" s="177" t="e">
+      <c r="B42" s="176" t="e">
         <f aca="false">IF(OR(A42=0,A42= " ")," ",IF(ISERROR(VLOOKUP(A42,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A42,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A42,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A42,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C42" s="178"/>
-      <c r="D42" s="179"/>
-      <c r="E42" s="180"/>
+      <c r="C42" s="177"/>
+      <c r="D42" s="178"/>
+      <c r="E42" s="179"/>
     </row>
     <row r="43" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="176" t="str">
+      <c r="A43" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A43 = " ",'ZE-Sum'!A43 = 0), " ", 'ZE-Sum'!A43)</f>
         <v> </v>
       </c>
-      <c r="B43" s="177" t="e">
+      <c r="B43" s="176" t="e">
         <f aca="false">IF(OR(A43=0,A43= " ")," ",IF(ISERROR(VLOOKUP(A43,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A43,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A43,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A43,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C43" s="178"/>
-      <c r="D43" s="179"/>
-      <c r="E43" s="180"/>
+      <c r="C43" s="177"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="179"/>
     </row>
     <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="176" t="str">
+      <c r="A44" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A44 = " ",'ZE-Sum'!A44 = 0), " ", 'ZE-Sum'!A44)</f>
         <v> </v>
       </c>
-      <c r="B44" s="177" t="e">
+      <c r="B44" s="176" t="e">
         <f aca="false">IF(OR(A44=0,A44= " ")," ",IF(ISERROR(VLOOKUP(A44,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A44,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A44,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A44,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C44" s="178"/>
-      <c r="D44" s="179"/>
-      <c r="E44" s="180"/>
+      <c r="C44" s="177"/>
+      <c r="D44" s="178"/>
+      <c r="E44" s="179"/>
     </row>
     <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="176" t="str">
+      <c r="A45" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A45 = " ",'ZE-Sum'!A45 = 0), " ", 'ZE-Sum'!A45)</f>
         <v> </v>
       </c>
-      <c r="B45" s="177" t="e">
+      <c r="B45" s="176" t="e">
         <f aca="false">IF(OR(A45=0,A45= " ")," ",IF(ISERROR(VLOOKUP(A45,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A45,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A45,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A45,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C45" s="178"/>
-      <c r="D45" s="179"/>
-      <c r="E45" s="180"/>
+      <c r="C45" s="177"/>
+      <c r="D45" s="178"/>
+      <c r="E45" s="179"/>
     </row>
     <row r="46" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="176" t="str">
+      <c r="A46" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A46 = " ",'ZE-Sum'!A46 = 0), " ", 'ZE-Sum'!A46)</f>
         <v> </v>
       </c>
-      <c r="B46" s="177" t="e">
+      <c r="B46" s="176" t="e">
         <f aca="false">IF(OR(A46=0,A46= " ")," ",IF(ISERROR(VLOOKUP(A46,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A46,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A46,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A46,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C46" s="178"/>
-      <c r="D46" s="179"/>
-      <c r="E46" s="180"/>
+      <c r="C46" s="177"/>
+      <c r="D46" s="178"/>
+      <c r="E46" s="179"/>
     </row>
     <row r="47" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="176" t="str">
+      <c r="A47" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A47 = " ",'ZE-Sum'!A47 = 0), " ", 'ZE-Sum'!A47)</f>
         <v> </v>
       </c>
-      <c r="B47" s="177" t="e">
+      <c r="B47" s="176" t="e">
         <f aca="false">IF(OR(A47=0,A47= " ")," ",IF(ISERROR(VLOOKUP(A47,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A47,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A47,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A47,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C47" s="178"/>
-      <c r="D47" s="179"/>
-      <c r="E47" s="180"/>
+      <c r="C47" s="177"/>
+      <c r="D47" s="178"/>
+      <c r="E47" s="179"/>
     </row>
     <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="176" t="str">
+      <c r="A48" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A48 = " ",'ZE-Sum'!A48 = 0), " ", 'ZE-Sum'!A48)</f>
         <v> </v>
       </c>
-      <c r="B48" s="177" t="e">
+      <c r="B48" s="176" t="e">
         <f aca="false">IF(OR(A48=0,A48= " ")," ",IF(ISERROR(VLOOKUP(A48,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A48,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A48,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A48,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C48" s="178"/>
-      <c r="D48" s="179"/>
-      <c r="E48" s="180"/>
+      <c r="C48" s="177"/>
+      <c r="D48" s="178"/>
+      <c r="E48" s="179"/>
     </row>
     <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="176" t="str">
+      <c r="A49" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A49 = " ",'ZE-Sum'!A49 = 0), " ", 'ZE-Sum'!A49)</f>
         <v> </v>
       </c>
-      <c r="B49" s="177" t="e">
+      <c r="B49" s="176" t="e">
         <f aca="false">IF(OR(A49=0,A49= " ")," ",IF(ISERROR(VLOOKUP(A49,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A49,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A49,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A49,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C49" s="178"/>
-      <c r="D49" s="179"/>
-      <c r="E49" s="180"/>
+      <c r="C49" s="177"/>
+      <c r="D49" s="178"/>
+      <c r="E49" s="179"/>
     </row>
     <row r="50" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="176" t="str">
+      <c r="A50" s="175" t="str">
         <f aca="false">IF(OR('ZE-Sum'!A50 = " ",'ZE-Sum'!A50 = 0), " ", 'ZE-Sum'!A50)</f>
         <v> </v>
       </c>
-      <c r="B50" s="177" t="e">
+      <c r="B50" s="176" t="e">
         <f aca="false">IF(OR(A50=0,A50= " ")," ",IF(ISERROR(VLOOKUP(A50,'ZE-Sum'!$A$8:$B$60,2,0)),IF(ISERROR(VLOOKUP(A50,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),"Achtung! FEHLER! Kostenstelle prüfen!",VLOOKUP(A50,'ZE-Sum'!$J$9:'ze-sum'!#ref!,2,0)),VLOOKUP(A50,'ZE-Sum'!$A$8:$B$60,2,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C50" s="178"/>
-      <c r="D50" s="179"/>
-      <c r="E50" s="180"/>
+      <c r="C50" s="177"/>
+      <c r="D50" s="178"/>
+      <c r="E50" s="179"/>
     </row>
     <row r="51" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="181"/>
-      <c r="B51" s="182" t="str">
+      <c r="A51" s="180"/>
+      <c r="B51" s="181" t="str">
         <f aca="false">IF(ZE!C3="DE","Summe Kostenstellen",IF(ZE!C3="EN","Total amount","---"))</f>
         <v>Summe Kostenstellen</v>
       </c>
-      <c r="C51" s="108" t="n">
+      <c r="C51" s="107" t="n">
         <f aca="false">SUM(C8:C50)</f>
         <v>15</v>
       </c>
-      <c r="D51" s="108" t="n">
+      <c r="D51" s="107" t="n">
         <f aca="false">SUM(D8:D50)</f>
         <v>20</v>
       </c>
-      <c r="E51" s="110" t="n">
+      <c r="E51" s="109" t="n">
         <f aca="false">SUM(E8:E50)</f>
         <v>20</v>
       </c>

</xml_diff>